<commit_message>
changing the import to work with existing data in the database
</commit_message>
<xml_diff>
--- a/TravelEditor/Data/imported_data.xlsx
+++ b/TravelEditor/Data/imported_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9230" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9230" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Trips" sheetId="1" r:id="rId1"/>
@@ -51,24 +51,12 @@
     <t>probno putovanje</t>
   </si>
   <si>
-    <t>{"DestinationId":1,"City":"Paris","Country":"France"}</t>
-  </si>
-  <si>
-    <t>[{"TravellerId":3,"Email":"mika@gmail.com","FirstName":"mika"}]</t>
-  </si>
-  <si>
-    <t>[{"ReviewId":11,"Comment":"aq","Rating":10}]</t>
-  </si>
-  <si>
     <t>putovanje2</t>
   </si>
   <si>
     <t>neki opisss</t>
   </si>
   <si>
-    <t>{"DestinationId":5,"City":"nova Destinacija","Country":"novann"}</t>
-  </si>
-  <si>
     <t>[]</t>
   </si>
   <si>
@@ -267,7 +255,19 @@
     <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
   </si>
   <si>
-    <t>{"TravellerId":3,"Email":"mika@gmail.com","FirstName":"mika"}</t>
+    <t>[{"TravellerId"108,"Email":"mika@gmail.com","FirstName":"mika"}]</t>
+  </si>
+  <si>
+    <t>{"TravellerId":108,"Email":"mika@gmail.com","FirstName":"mika"}</t>
+  </si>
+  <si>
+    <t>[{"ReviewId":35,"Comment":"aq","Rating":10}]</t>
+  </si>
+  <si>
+    <t>{"DestinationId":110,"City":"Paris","Country":"France"}</t>
+  </si>
+  <si>
+    <t>{"DestinationId":112,"City":"nova Destinacija","Country":"novann"}</t>
   </si>
 </sst>
 </file>
@@ -679,7 +679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -720,7 +722,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -735,21 +737,21 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>45637</v>
@@ -758,24 +760,24 @@
         <v>45640</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>45870</v>
@@ -784,16 +786,16 @@
         <v>45879</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -807,7 +809,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -822,82 +824,82 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -910,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -925,7 +927,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -934,78 +936,78 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D5">
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1018,7 +1020,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1032,39 +1036,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F2">
         <v>34</v>
@@ -1072,39 +1076,39 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F3">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F4">
         <v>20</v>
@@ -1136,30 +1140,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
         <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1171,7 +1175,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1190,42 +1194,42 @@
   <sheetData>
     <row r="1" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring services for import and export
</commit_message>
<xml_diff>
--- a/TravelEditor/Data/imported_data.xlsx
+++ b/TravelEditor/Data/imported_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Trips" sheetId="1" r:id="rId1"/>
@@ -14,16 +14,12 @@
     <sheet name="Reviews" sheetId="5" r:id="rId5"/>
     <sheet name="Evaluation Warning" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="4294901760"/>
 </workbook>
 </file>
 
-<file path=xl/cellimages.xml>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
   <si>
     <t>TripId</t>
   </si>
@@ -139,9 +135,6 @@
     <t>novann</t>
   </si>
   <si>
-    <t>nova</t>
-  </si>
-  <si>
     <t>novaaa</t>
   </si>
   <si>
@@ -157,9 +150,6 @@
     <t>cold,rainy</t>
   </si>
   <si>
-    <t>[{"AttractionId":181,"Name":"London Bridge"}]</t>
-  </si>
-  <si>
     <t>AttractionId</t>
   </si>
   <si>
@@ -299,16 +289,41 @@
   </si>
   <si>
     <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
+  </si>
+  <si>
+    <t>nova opis opis</t>
+  </si>
+  <si>
+    <t>zika</t>
+  </si>
+  <si>
+    <t>zikic</t>
+  </si>
+  <si>
+    <t>zika@gmail.com</t>
+  </si>
+  <si>
+    <t>London Eye</t>
+  </si>
+  <si>
+    <t>[{"AttractionId":181,"Name":"London Bridge"},{"AttractionId":192,"Name":"London Eye"}]</t>
+  </si>
+  <si>
+    <t>A wheel in London that looks like an eye</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="dd-MMM-yy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -321,16 +336,21 @@
       <family val="2"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -345,122 +365,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
+  <cellStyleXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20">
-      <alignment/>
-      <protection/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0"/>
-    <cellStyle name="Percent" xfId="15"/>
-    <cellStyle name="Currency" xfId="16"/>
-    <cellStyle name="Currency [0]" xfId="17"/>
-    <cellStyle name="Comma" xfId="18"/>
-    <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="20"/>
+    <cellStyle name="Comma" xfId="4"/>
+    <cellStyle name="Comma [0]" xfId="5"/>
+    <cellStyle name="Currency" xfId="2"/>
+    <cellStyle name="Currency [0]" xfId="3"/>
+    <cellStyle name="Hyperlink" xfId="6"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -783,23 +719,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" widthPt="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.00390625" widthPt="52.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.7109375" widthPt="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" widthPt="79.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.00390625" widthPt="288.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="110.140625" widthPt="578.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="75.28125" widthPt="395.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="110.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="75.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -825,7 +761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>90</v>
       </c>
@@ -851,7 +787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>91</v>
       </c>
@@ -877,7 +813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>92</v>
       </c>
@@ -904,29 +840,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.00390625" widthPt="63" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" widthPt="77.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.00390625" widthPt="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.00390625" widthPt="351.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" widthPt="84.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="76.7109375" widthPt="402.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="76.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -946,7 +883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12.75">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>110</v>
       </c>
@@ -966,7 +903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="12.75">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>111</v>
       </c>
@@ -986,7 +923,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.75">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>112</v>
       </c>
@@ -997,60 +934,61 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
         <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.75">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>113</v>
       </c>
       <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" widthPt="56.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.57421875" widthPt="102.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.28125" widthPt="437.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.57421875" widthPt="29.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.28125" widthPt="264" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1059,232 +997,272 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="12.75">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2">
         <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="12.75">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="12.75">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>192</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.421875" widthPt="49.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.8515625" widthPt="51.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" widthPt="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" widthPt="82.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.00390625" widthPt="68.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.57421875" widthPt="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="12.75">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>108</v>
       </c>
       <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
       <c r="F2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="12.75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>109</v>
       </c>
       <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F3">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.75">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4">
         <v>20</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5">
+        <v>12432</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions/>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.421875" widthPt="44.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28125" widthPt="48.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.57421875" widthPt="34.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" widthPt="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.421875" widthPt="49.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.28125" widthPt="290.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="12.75">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1296,15 +1274,15 @@
         <v>108</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="12.75">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -1316,15 +1294,15 @@
         <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="12.75">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -1336,72 +1314,70 @@
         <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" ht="12.75">
+    <row r="1" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" ht="12.75">
-      <c r="B2" s="2" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" ht="12.75">
-      <c r="B4" t="s">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" ht="12.75">
-      <c r="B5" s="4" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" ht="12.75">
-      <c r="B7" t="s">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" ht="12.75">
-      <c r="B8" s="4" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="10" ht="12.75">
-      <c r="B10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" ht="12.75">
-      <c r="B11" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://www.e-iceblue.com"/>
-    <hyperlink ref="B8" r:id="rId2" display="mailto:support@e-iceblue.com"/>
-    <hyperlink ref="B11" r:id="rId3" display="https://www.e-iceblue.com/Buy/Spire.XLS.html"/>
+    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId3"/>
   </hyperlinks>
-  <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding tests and improving import logic
</commit_message>
<xml_diff>
--- a/TravelEditor/Data/imported_data.xlsx
+++ b/TravelEditor/Data/imported_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9230" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9230"/>
   </bookViews>
   <sheets>
     <sheet name="Trips" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
   <si>
     <t>TripId</t>
   </si>
@@ -54,9 +54,6 @@
     <t>{"DestinationId":110,"City":"Paris","Country":"France"}</t>
   </si>
   <si>
-    <t>[{"TravellerId":108,"Email":"mika@gmail.com","FirstName":"mika"},{"TravellerId":109,"Email":"pera@gmail.com","FirstName":"pera"}]</t>
-  </si>
-  <si>
     <t>[{"ReviewId":35,"Comment":"aq","Rating":10},{"ReviewId":36,"Comment":"pp","Rating":10}]</t>
   </si>
   <si>
@@ -66,15 +63,9 @@
     <t>neki opisss</t>
   </si>
   <si>
-    <t>{"DestinationId":112,"City":"nova Destinacija","Country":"novann"}</t>
-  </si>
-  <si>
     <t>[{"TravellerId":110,"Email":"test@gmail.com","FirstName":"jedan"}]</t>
   </si>
   <si>
-    <t>[{"ReviewId":42,"Comment":"pp","Rating":10}]</t>
-  </si>
-  <si>
     <t>w</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>Cold,</t>
   </si>
   <si>
-    <t>[{"AttractionId":175,"Name":"Notre Dame Cathedral"}]</t>
-  </si>
-  <si>
     <t>New York</t>
   </si>
   <si>
@@ -132,9 +120,6 @@
     <t>nova Destinacija</t>
   </si>
   <si>
-    <t>novann</t>
-  </si>
-  <si>
     <t>novaaa</t>
   </si>
   <si>
@@ -310,6 +295,18 @@
   </si>
   <si>
     <t>A wheel in London that looks like an eye</t>
+  </si>
+  <si>
+    <t>Nova drzava</t>
+  </si>
+  <si>
+    <t>[{"TravellerId":108,"Email":"mika@gmail.com","FirstName":"mika"}]</t>
+  </si>
+  <si>
+    <t>{"DestinationId":113,"City":"London","Country":"England"}</t>
+  </si>
+  <si>
+    <t>{"DestinationId":112,"City":"nova Destinacija","Country":"Nova drzava"}</t>
   </si>
 </sst>
 </file>
@@ -722,7 +719,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -781,10 +780,10 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -792,7 +791,7 @@
         <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>45271</v>
@@ -801,13 +800,13 @@
         <v>45274</v>
       </c>
       <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
@@ -818,7 +817,7 @@
         <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>45870</v>
@@ -827,16 +826,16 @@
         <v>45879</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -849,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -865,22 +864,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -888,19 +887,19 @@
         <v>110</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -908,19 +907,19 @@
         <v>111</v>
       </c>
       <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
         <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -928,19 +927,19 @@
         <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -948,19 +947,19 @@
         <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -988,7 +987,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -997,10 +996,10 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1008,16 +1007,16 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1025,16 +1024,16 @@
         <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1042,16 +1041,16 @@
         <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1059,16 +1058,16 @@
         <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1076,16 +1075,16 @@
         <v>192</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D6">
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1114,22 +1113,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
         <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1137,16 +1136,16 @@
         <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F2">
         <v>22</v>
@@ -1157,16 +1156,16 @@
         <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F3">
         <v>29</v>
@@ -1177,16 +1176,16 @@
         <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F4">
         <v>20</v>
@@ -1197,13 +1196,13 @@
         <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E5">
         <v>12432</v>
@@ -1239,22 +1238,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1262,7 +1261,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1274,7 +1273,7 @@
         <v>108</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1282,7 +1281,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -1294,7 +1293,7 @@
         <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1302,7 +1301,7 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -1314,7 +1313,7 @@
         <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1333,42 +1332,42 @@
   <sheetData>
     <row r="1" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>